<commit_message>
differ optimisation and plots
</commit_message>
<xml_diff>
--- a/Comsol/Task/Table for SOR.xlsx
+++ b/Comsol/Task/Table for SOR.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20397"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WORKS\PolimerSolve\Comsol\Task\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Works\PolimerSolve\Comsol\Task\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{166AF85D-9B83-49A4-94F9-73774458B2A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E344FF47-A705-4D21-B5AE-DA78B9C3313B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60FE5ACB-4118-41CB-AB65-5BEC2C35F150}"/>
   </bookViews>
@@ -29,12 +29,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2839,7 +2833,7 @@
   <dimension ref="A1:C60"/>
   <sheetViews>
     <sheetView zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2852,9 +2846,9 @@
         <f>IFERROR(LEFT(R_input!$B1,FIND("*",R_input!$B1)-1),"")</f>
         <v xml:space="preserve"> k1</v>
       </c>
-      <c r="B1" s="4">
-        <f>IF(R_input!$C1=0,"",R_input!$C1)</f>
-        <v>10000</v>
+      <c r="B1" s="4" t="str">
+        <f>IF('C'!$A1="","",'C'!$A1&amp;"init")</f>
+        <v xml:space="preserve"> k1init</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -2862,9 +2856,9 @@
         <f>IFERROR(LEFT(R_input!$B2,FIND("*",R_input!$B2)-1),"")</f>
         <v xml:space="preserve"> k2</v>
       </c>
-      <c r="B2" s="4">
-        <f>IF(R_input!$C2=0,"",R_input!$C2)</f>
-        <v>10000</v>
+      <c r="B2" s="4" t="str">
+        <f>IF('C'!$A2="","",'C'!$A2&amp;"init")</f>
+        <v xml:space="preserve"> k2init</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -2872,9 +2866,9 @@
         <f>IFERROR(LEFT(R_input!$B3,FIND("*",R_input!$B3)-1),"")</f>
         <v xml:space="preserve"> k3</v>
       </c>
-      <c r="B3" s="4">
-        <f>IF(R_input!$C3=0,"",R_input!$C3)</f>
-        <v>100</v>
+      <c r="B3" s="4" t="str">
+        <f>IF('C'!$A3="","",'C'!$A3&amp;"init")</f>
+        <v xml:space="preserve"> k3init</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -2883,8 +2877,8 @@
         <v xml:space="preserve"> k4</v>
       </c>
       <c r="B4" s="4" t="str">
-        <f>IF(R_input!$C4=0,"",R_input!$C4)</f>
-        <v>K2*k5</v>
+        <f>IF('C'!$A4="","",'C'!$A4&amp;"init")</f>
+        <v xml:space="preserve"> k4init</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -2892,9 +2886,9 @@
         <f>IFERROR(LEFT(R_input!$B5,FIND("*",R_input!$B5)-1),"")</f>
         <v xml:space="preserve"> k5</v>
       </c>
-      <c r="B5" s="4">
-        <f>IF(R_input!$C5=0,"",R_input!$C5)</f>
-        <v>1E-4</v>
+      <c r="B5" s="4" t="str">
+        <f>IF('C'!$A5="","",'C'!$A5&amp;"init")</f>
+        <v xml:space="preserve"> k5init</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -2902,9 +2896,9 @@
         <f>IFERROR(LEFT(R_input!$B6,FIND("*",R_input!$B6)-1),"")</f>
         <v xml:space="preserve"> k6</v>
       </c>
-      <c r="B6" s="4">
-        <f>IF(R_input!$C6=0,"",R_input!$C6)</f>
-        <v>2</v>
+      <c r="B6" s="4" t="str">
+        <f>IF('C'!$A6="","",'C'!$A6&amp;"init")</f>
+        <v xml:space="preserve"> k6init</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -2913,8 +2907,8 @@
         <v xml:space="preserve"> k7</v>
       </c>
       <c r="B7" s="4" t="str">
-        <f>IF(R_input!$C7=0,"",R_input!$C7)</f>
-        <v>K4*k8</v>
+        <f>IF('C'!$A7="","",'C'!$A7&amp;"init")</f>
+        <v xml:space="preserve"> k7init</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -2922,9 +2916,9 @@
         <f>IFERROR(LEFT(R_input!$B8,FIND("*",R_input!$B8)-1),"")</f>
         <v xml:space="preserve"> k8</v>
       </c>
-      <c r="B8" s="4">
-        <f>IF(R_input!$C8=0,"",R_input!$C8)</f>
-        <v>1</v>
+      <c r="B8" s="4" t="str">
+        <f>IF('C'!$A8="","",'C'!$A8&amp;"init")</f>
+        <v xml:space="preserve"> k8init</v>
       </c>
       <c r="C8" s="10"/>
     </row>
@@ -2933,9 +2927,9 @@
         <f>IFERROR(LEFT(R_input!$B9,FIND("*",R_input!$B9)-1),"")</f>
         <v xml:space="preserve"> k9</v>
       </c>
-      <c r="B9" s="4">
-        <f>IF(R_input!$C9=0,"",R_input!$C9)</f>
-        <v>1</v>
+      <c r="B9" s="4" t="str">
+        <f>IF('C'!$A9="","",'C'!$A9&amp;"init")</f>
+        <v xml:space="preserve"> k9init</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -2943,9 +2937,9 @@
         <f>IFERROR(LEFT(R_input!$B10,FIND("*",R_input!$B10)-1),"")</f>
         <v xml:space="preserve"> k10</v>
       </c>
-      <c r="B10" s="4">
-        <f>IF(R_input!$C10=0,"",R_input!$C10)</f>
-        <v>10</v>
+      <c r="B10" s="4" t="str">
+        <f>IF('C'!$A10="","",'C'!$A10&amp;"init")</f>
+        <v xml:space="preserve"> k10init</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -2953,9 +2947,9 @@
         <f>IFERROR(LEFT(R_input!$B11,FIND("*",R_input!$B11)-1),"")</f>
         <v xml:space="preserve"> k11</v>
       </c>
-      <c r="B11" s="4">
-        <f>IF(R_input!$C11=0,"",R_input!$C11)</f>
-        <v>1</v>
+      <c r="B11" s="4" t="str">
+        <f>IF('C'!$A11="","",'C'!$A11&amp;"init")</f>
+        <v xml:space="preserve"> k11init</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -2963,9 +2957,9 @@
         <f>IFERROR(LEFT(R_input!$B12,FIND("*",R_input!$B12)-1),"")</f>
         <v>K2</v>
       </c>
-      <c r="B12" s="4">
-        <f>IF(R_input!$C12=0,"",R_input!$C12)</f>
-        <v>100000</v>
+      <c r="B12" s="4" t="str">
+        <f>IF('C'!$A12="","",'C'!$A12&amp;"init")</f>
+        <v>K2init</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -2973,9 +2967,9 @@
         <f>IFERROR(LEFT(R_input!$B13,FIND("*",R_input!$B13)-1),"")</f>
         <v>K4</v>
       </c>
-      <c r="B13" s="4">
-        <f>IF(R_input!$C13=0,"",R_input!$C13)</f>
-        <v>0.05</v>
+      <c r="B13" s="4" t="str">
+        <f>IF('C'!$A13="","",'C'!$A13&amp;"init")</f>
+        <v>K4init</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -2984,7 +2978,7 @@
         <v/>
       </c>
       <c r="B14" s="4" t="str">
-        <f>IF(R_input!$C14=0,"",R_input!$C14)</f>
+        <f>IF('C'!$A14="","",'C'!$A14&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -2994,7 +2988,7 @@
         <v/>
       </c>
       <c r="B15" s="4" t="str">
-        <f>IF(R_input!$C15=0,"",R_input!$C15)</f>
+        <f>IF('C'!$A15="","",'C'!$A15&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3004,7 +2998,7 @@
         <v/>
       </c>
       <c r="B16" s="4" t="str">
-        <f>IF(R_input!$C16=0,"",R_input!$C16)</f>
+        <f>IF('C'!$A16="","",'C'!$A16&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3014,7 +3008,7 @@
         <v/>
       </c>
       <c r="B17" s="4" t="str">
-        <f>IF(R_input!$C17=0,"",R_input!$C17)</f>
+        <f>IF('C'!$A17="","",'C'!$A17&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3024,7 +3018,7 @@
         <v/>
       </c>
       <c r="B18" s="4" t="str">
-        <f>IF(R_input!$C18=0,"",R_input!$C18)</f>
+        <f>IF('C'!$A18="","",'C'!$A18&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3034,7 +3028,7 @@
         <v/>
       </c>
       <c r="B19" s="4" t="str">
-        <f>IF(R_input!$C19=0,"",R_input!$C19)</f>
+        <f>IF('C'!$A19="","",'C'!$A19&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3044,7 +3038,7 @@
         <v/>
       </c>
       <c r="B20" s="4" t="str">
-        <f>IF(R_input!$C20=0,"",R_input!$C20)</f>
+        <f>IF('C'!$A20="","",'C'!$A20&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3054,7 +3048,7 @@
         <v/>
       </c>
       <c r="B21" s="4" t="str">
-        <f>IF(R_input!$C21=0,"",R_input!$C21)</f>
+        <f>IF('C'!$A21="","",'C'!$A21&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3064,7 +3058,7 @@
         <v/>
       </c>
       <c r="B22" s="4" t="str">
-        <f>IF(R_input!$C22=0,"",R_input!$C22)</f>
+        <f>IF('C'!$A22="","",'C'!$A22&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3074,7 +3068,7 @@
         <v/>
       </c>
       <c r="B23" s="4" t="str">
-        <f>IF(R_input!$C23=0,"",R_input!$C23)</f>
+        <f>IF('C'!$A23="","",'C'!$A23&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3084,7 +3078,7 @@
         <v/>
       </c>
       <c r="B24" s="4" t="str">
-        <f>IF(R_input!$C24=0,"",R_input!$C24)</f>
+        <f>IF('C'!$A24="","",'C'!$A24&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3094,7 +3088,7 @@
         <v/>
       </c>
       <c r="B25" s="4" t="str">
-        <f>IF(R_input!$C25=0,"",R_input!$C25)</f>
+        <f>IF('C'!$A25="","",'C'!$A25&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3104,7 +3098,7 @@
         <v/>
       </c>
       <c r="B26" s="4" t="str">
-        <f>IF(R_input!$C26=0,"",R_input!$C26)</f>
+        <f>IF('C'!$A26="","",'C'!$A26&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3114,7 +3108,7 @@
         <v/>
       </c>
       <c r="B27" s="4" t="str">
-        <f>IF(R_input!$C27=0,"",R_input!$C27)</f>
+        <f>IF('C'!$A27="","",'C'!$A27&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3124,7 +3118,7 @@
         <v/>
       </c>
       <c r="B28" s="4" t="str">
-        <f>IF(R_input!$C28=0,"",R_input!$C28)</f>
+        <f>IF('C'!$A28="","",'C'!$A28&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3134,7 +3128,7 @@
         <v/>
       </c>
       <c r="B29" s="4" t="str">
-        <f>IF(R_input!$C29=0,"",R_input!$C29)</f>
+        <f>IF('C'!$A29="","",'C'!$A29&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3144,7 +3138,7 @@
         <v/>
       </c>
       <c r="B30" s="4" t="str">
-        <f>IF(R_input!$C30=0,"",R_input!$C30)</f>
+        <f>IF('C'!$A30="","",'C'!$A30&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3154,7 +3148,7 @@
         <v/>
       </c>
       <c r="B31" s="4" t="str">
-        <f>IF(R_input!$C31=0,"",R_input!$C31)</f>
+        <f>IF('C'!$A31="","",'C'!$A31&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3164,7 +3158,7 @@
         <v/>
       </c>
       <c r="B32" s="4" t="str">
-        <f>IF(R_input!$C32=0,"",R_input!$C32)</f>
+        <f>IF('C'!$A32="","",'C'!$A32&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3174,7 +3168,7 @@
         <v/>
       </c>
       <c r="B33" s="4" t="str">
-        <f>IF(R_input!$C33=0,"",R_input!$C33)</f>
+        <f>IF('C'!$A33="","",'C'!$A33&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3184,7 +3178,7 @@
         <v/>
       </c>
       <c r="B34" s="4" t="str">
-        <f>IF(R_input!$C34=0,"",R_input!$C34)</f>
+        <f>IF('C'!$A34="","",'C'!$A34&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3194,7 +3188,7 @@
         <v/>
       </c>
       <c r="B35" s="4" t="str">
-        <f>IF(R_input!$C35=0,"",R_input!$C35)</f>
+        <f>IF('C'!$A35="","",'C'!$A35&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3204,7 +3198,7 @@
         <v/>
       </c>
       <c r="B36" s="4" t="str">
-        <f>IF(R_input!$C36=0,"",R_input!$C36)</f>
+        <f>IF('C'!$A36="","",'C'!$A36&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3214,7 +3208,7 @@
         <v/>
       </c>
       <c r="B37" s="4" t="str">
-        <f>IF(R_input!$C37=0,"",R_input!$C37)</f>
+        <f>IF('C'!$A37="","",'C'!$A37&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3224,7 +3218,7 @@
         <v/>
       </c>
       <c r="B38" s="4" t="str">
-        <f>IF(R_input!$C38=0,"",R_input!$C38)</f>
+        <f>IF('C'!$A38="","",'C'!$A38&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3234,7 +3228,7 @@
         <v/>
       </c>
       <c r="B39" s="4" t="str">
-        <f>IF(R_input!$C39=0,"",R_input!$C39)</f>
+        <f>IF('C'!$A39="","",'C'!$A39&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3244,7 +3238,7 @@
         <v/>
       </c>
       <c r="B40" s="4" t="str">
-        <f>IF(R_input!$C40=0,"",R_input!$C40)</f>
+        <f>IF('C'!$A40="","",'C'!$A40&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3254,7 +3248,7 @@
         <v/>
       </c>
       <c r="B41" s="4" t="str">
-        <f>IF(R_input!$C41=0,"",R_input!$C41)</f>
+        <f>IF('C'!$A41="","",'C'!$A41&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3264,7 +3258,7 @@
         <v/>
       </c>
       <c r="B42" s="4" t="str">
-        <f>IF(R_input!$C42=0,"",R_input!$C42)</f>
+        <f>IF('C'!$A42="","",'C'!$A42&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3274,7 +3268,7 @@
         <v/>
       </c>
       <c r="B43" s="4" t="str">
-        <f>IF(R_input!$C43=0,"",R_input!$C43)</f>
+        <f>IF('C'!$A43="","",'C'!$A43&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3284,7 +3278,7 @@
         <v/>
       </c>
       <c r="B44" s="4" t="str">
-        <f>IF(R_input!$C44=0,"",R_input!$C44)</f>
+        <f>IF('C'!$A44="","",'C'!$A44&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3294,7 +3288,7 @@
         <v/>
       </c>
       <c r="B45" s="4" t="str">
-        <f>IF(R_input!$C45=0,"",R_input!$C45)</f>
+        <f>IF('C'!$A45="","",'C'!$A45&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3304,7 +3298,7 @@
         <v/>
       </c>
       <c r="B46" s="4" t="str">
-        <f>IF(R_input!$C46=0,"",R_input!$C46)</f>
+        <f>IF('C'!$A46="","",'C'!$A46&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3314,7 +3308,7 @@
         <v/>
       </c>
       <c r="B47" s="4" t="str">
-        <f>IF(R_input!$C47=0,"",R_input!$C47)</f>
+        <f>IF('C'!$A47="","",'C'!$A47&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3324,7 +3318,7 @@
         <v/>
       </c>
       <c r="B48" s="4" t="str">
-        <f>IF(R_input!$C48=0,"",R_input!$C48)</f>
+        <f>IF('C'!$A48="","",'C'!$A48&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3334,7 +3328,7 @@
         <v/>
       </c>
       <c r="B49" s="4" t="str">
-        <f>IF(R_input!$C49=0,"",R_input!$C49)</f>
+        <f>IF('C'!$A49="","",'C'!$A49&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3344,7 +3338,7 @@
         <v/>
       </c>
       <c r="B50" s="4" t="str">
-        <f>IF(R_input!$C50=0,"",R_input!$C50)</f>
+        <f>IF('C'!$A50="","",'C'!$A50&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3354,7 +3348,7 @@
         <v/>
       </c>
       <c r="B51" s="4" t="str">
-        <f>IF(R_input!$C51=0,"",R_input!$C51)</f>
+        <f>IF('C'!$A51="","",'C'!$A51&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3364,7 +3358,7 @@
         <v/>
       </c>
       <c r="B52" s="4" t="str">
-        <f>IF(R_input!$C52=0,"",R_input!$C52)</f>
+        <f>IF('C'!$A52="","",'C'!$A52&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3374,7 +3368,7 @@
         <v/>
       </c>
       <c r="B53" s="4" t="str">
-        <f>IF(R_input!$C53=0,"",R_input!$C53)</f>
+        <f>IF('C'!$A53="","",'C'!$A53&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3384,7 +3378,7 @@
         <v/>
       </c>
       <c r="B54" s="4" t="str">
-        <f>IF(R_input!$C54=0,"",R_input!$C54)</f>
+        <f>IF('C'!$A54="","",'C'!$A54&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3394,7 +3388,7 @@
         <v/>
       </c>
       <c r="B55" s="4" t="str">
-        <f>IF(R_input!$C55=0,"",R_input!$C55)</f>
+        <f>IF('C'!$A55="","",'C'!$A55&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3404,7 +3398,7 @@
         <v/>
       </c>
       <c r="B56" s="4" t="str">
-        <f>IF(R_input!$C56=0,"",R_input!$C56)</f>
+        <f>IF('C'!$A56="","",'C'!$A56&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3414,7 +3408,7 @@
         <v/>
       </c>
       <c r="B57" s="4" t="str">
-        <f>IF(R_input!$C57=0,"",R_input!$C57)</f>
+        <f>IF('C'!$A57="","",'C'!$A57&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3424,7 +3418,7 @@
         <v/>
       </c>
       <c r="B58" s="4" t="str">
-        <f>IF(R_input!$C58=0,"",R_input!$C58)</f>
+        <f>IF('C'!$A58="","",'C'!$A58&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3434,7 +3428,7 @@
         <v/>
       </c>
       <c r="B59" s="4" t="str">
-        <f>IF(R_input!$C59=0,"",R_input!$C59)</f>
+        <f>IF('C'!$A59="","",'C'!$A59&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3444,7 +3438,7 @@
         <v/>
       </c>
       <c r="B60" s="4" t="str">
-        <f>IF(R_input!$C60=0,"",R_input!$C60)</f>
+        <f>IF('C'!$A60="","",'C'!$A60&amp;"init")</f>
         <v/>
       </c>
     </row>
@@ -3458,7 +3452,7 @@
   <dimension ref="A1:B60"/>
   <sheetViews>
     <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3469,7 +3463,7 @@
         <v xml:space="preserve"> k1init</v>
       </c>
       <c r="B1" s="4">
-        <f>'C'!$B1</f>
+        <f>IF(R_input!$C1=0,"",R_input!$C1)</f>
         <v>10000</v>
       </c>
     </row>
@@ -3479,7 +3473,7 @@
         <v xml:space="preserve"> k2init</v>
       </c>
       <c r="B2" s="4">
-        <f>'C'!$B2</f>
+        <f>IF(R_input!$C2=0,"",R_input!$C2)</f>
         <v>10000</v>
       </c>
     </row>
@@ -3489,7 +3483,7 @@
         <v xml:space="preserve"> k3init</v>
       </c>
       <c r="B3" s="4">
-        <f>'C'!$B3</f>
+        <f>IF(R_input!$C3=0,"",R_input!$C3)</f>
         <v>100</v>
       </c>
     </row>
@@ -3499,7 +3493,7 @@
         <v xml:space="preserve"> k4init</v>
       </c>
       <c r="B4" s="4" t="str">
-        <f>'C'!$B4</f>
+        <f>IF(R_input!$C4=0,"",R_input!$C4)</f>
         <v>K2*k5</v>
       </c>
     </row>
@@ -3509,7 +3503,7 @@
         <v xml:space="preserve"> k5init</v>
       </c>
       <c r="B5" s="4">
-        <f>'C'!$B5</f>
+        <f>IF(R_input!$C5=0,"",R_input!$C5)</f>
         <v>1E-4</v>
       </c>
     </row>
@@ -3519,7 +3513,7 @@
         <v xml:space="preserve"> k6init</v>
       </c>
       <c r="B6" s="4">
-        <f>'C'!$B6</f>
+        <f>IF(R_input!$C6=0,"",R_input!$C6)</f>
         <v>2</v>
       </c>
     </row>
@@ -3529,7 +3523,7 @@
         <v xml:space="preserve"> k7init</v>
       </c>
       <c r="B7" s="4" t="str">
-        <f>'C'!$B7</f>
+        <f>IF(R_input!$C7=0,"",R_input!$C7)</f>
         <v>K4*k8</v>
       </c>
     </row>
@@ -3539,7 +3533,7 @@
         <v xml:space="preserve"> k8init</v>
       </c>
       <c r="B8" s="4">
-        <f>'C'!$B8</f>
+        <f>IF(R_input!$C8=0,"",R_input!$C8)</f>
         <v>1</v>
       </c>
     </row>
@@ -3549,7 +3543,7 @@
         <v xml:space="preserve"> k9init</v>
       </c>
       <c r="B9" s="4">
-        <f>'C'!$B9</f>
+        <f>IF(R_input!$C9=0,"",R_input!$C9)</f>
         <v>1</v>
       </c>
     </row>
@@ -3559,7 +3553,7 @@
         <v xml:space="preserve"> k10init</v>
       </c>
       <c r="B10" s="4">
-        <f>'C'!$B10</f>
+        <f>IF(R_input!$C10=0,"",R_input!$C10)</f>
         <v>10</v>
       </c>
     </row>
@@ -3569,7 +3563,7 @@
         <v xml:space="preserve"> k11init</v>
       </c>
       <c r="B11" s="4">
-        <f>'C'!$B11</f>
+        <f>IF(R_input!$C11=0,"",R_input!$C11)</f>
         <v>1</v>
       </c>
     </row>
@@ -3579,7 +3573,7 @@
         <v>K2init</v>
       </c>
       <c r="B12" s="4">
-        <f>'C'!$B12</f>
+        <f>IF(R_input!$C12=0,"",R_input!$C12)</f>
         <v>100000</v>
       </c>
     </row>
@@ -3589,7 +3583,7 @@
         <v>K4init</v>
       </c>
       <c r="B13" s="4">
-        <f>'C'!$B13</f>
+        <f>IF(R_input!$C13=0,"",R_input!$C13)</f>
         <v>0.05</v>
       </c>
     </row>
@@ -3599,7 +3593,7 @@
         <v/>
       </c>
       <c r="B14" s="4" t="str">
-        <f>'C'!$B14</f>
+        <f>IF(R_input!$C14=0,"",R_input!$C14)</f>
         <v/>
       </c>
     </row>
@@ -3609,7 +3603,7 @@
         <v/>
       </c>
       <c r="B15" s="4" t="str">
-        <f>'C'!$B15</f>
+        <f>IF(R_input!$C15=0,"",R_input!$C15)</f>
         <v/>
       </c>
     </row>
@@ -3619,7 +3613,7 @@
         <v/>
       </c>
       <c r="B16" s="4" t="str">
-        <f>'C'!$B16</f>
+        <f>IF(R_input!$C16=0,"",R_input!$C16)</f>
         <v/>
       </c>
     </row>
@@ -3629,7 +3623,7 @@
         <v/>
       </c>
       <c r="B17" s="4" t="str">
-        <f>'C'!$B17</f>
+        <f>IF(R_input!$C17=0,"",R_input!$C17)</f>
         <v/>
       </c>
     </row>
@@ -3639,7 +3633,7 @@
         <v/>
       </c>
       <c r="B18" s="4" t="str">
-        <f>'C'!$B18</f>
+        <f>IF(R_input!$C18=0,"",R_input!$C18)</f>
         <v/>
       </c>
     </row>
@@ -3649,7 +3643,7 @@
         <v/>
       </c>
       <c r="B19" s="4" t="str">
-        <f>'C'!$B19</f>
+        <f>IF(R_input!$C19=0,"",R_input!$C19)</f>
         <v/>
       </c>
     </row>
@@ -3659,7 +3653,7 @@
         <v/>
       </c>
       <c r="B20" s="4" t="str">
-        <f>'C'!$B20</f>
+        <f>IF(R_input!$C20=0,"",R_input!$C20)</f>
         <v/>
       </c>
     </row>
@@ -3669,7 +3663,7 @@
         <v/>
       </c>
       <c r="B21" s="4" t="str">
-        <f>'C'!$B21</f>
+        <f>IF(R_input!$C21=0,"",R_input!$C21)</f>
         <v/>
       </c>
     </row>
@@ -3679,7 +3673,7 @@
         <v/>
       </c>
       <c r="B22" s="4" t="str">
-        <f>'C'!$B22</f>
+        <f>IF(R_input!$C22=0,"",R_input!$C22)</f>
         <v/>
       </c>
     </row>
@@ -3689,7 +3683,7 @@
         <v/>
       </c>
       <c r="B23" s="4" t="str">
-        <f>'C'!$B23</f>
+        <f>IF(R_input!$C23=0,"",R_input!$C23)</f>
         <v/>
       </c>
     </row>
@@ -3699,7 +3693,7 @@
         <v/>
       </c>
       <c r="B24" s="4" t="str">
-        <f>'C'!$B24</f>
+        <f>IF(R_input!$C24=0,"",R_input!$C24)</f>
         <v/>
       </c>
     </row>
@@ -3709,7 +3703,7 @@
         <v/>
       </c>
       <c r="B25" s="4" t="str">
-        <f>'C'!$B25</f>
+        <f>IF(R_input!$C25=0,"",R_input!$C25)</f>
         <v/>
       </c>
     </row>
@@ -3719,7 +3713,7 @@
         <v/>
       </c>
       <c r="B26" s="4" t="str">
-        <f>'C'!$B26</f>
+        <f>IF(R_input!$C26=0,"",R_input!$C26)</f>
         <v/>
       </c>
     </row>
@@ -3729,7 +3723,7 @@
         <v/>
       </c>
       <c r="B27" s="4" t="str">
-        <f>'C'!$B27</f>
+        <f>IF(R_input!$C27=0,"",R_input!$C27)</f>
         <v/>
       </c>
     </row>
@@ -3739,7 +3733,7 @@
         <v/>
       </c>
       <c r="B28" s="4" t="str">
-        <f>'C'!$B28</f>
+        <f>IF(R_input!$C28=0,"",R_input!$C28)</f>
         <v/>
       </c>
     </row>
@@ -3749,7 +3743,7 @@
         <v/>
       </c>
       <c r="B29" s="4" t="str">
-        <f>'C'!$B29</f>
+        <f>IF(R_input!$C29=0,"",R_input!$C29)</f>
         <v/>
       </c>
     </row>
@@ -3759,7 +3753,7 @@
         <v/>
       </c>
       <c r="B30" s="4" t="str">
-        <f>'C'!$B30</f>
+        <f>IF(R_input!$C30=0,"",R_input!$C30)</f>
         <v/>
       </c>
     </row>
@@ -3769,7 +3763,7 @@
         <v/>
       </c>
       <c r="B31" s="4" t="str">
-        <f>'C'!$B31</f>
+        <f>IF(R_input!$C31=0,"",R_input!$C31)</f>
         <v/>
       </c>
     </row>
@@ -3779,7 +3773,7 @@
         <v/>
       </c>
       <c r="B32" s="4" t="str">
-        <f>'C'!$B32</f>
+        <f>IF(R_input!$C32=0,"",R_input!$C32)</f>
         <v/>
       </c>
     </row>
@@ -3789,7 +3783,7 @@
         <v/>
       </c>
       <c r="B33" s="4" t="str">
-        <f>'C'!$B33</f>
+        <f>IF(R_input!$C33=0,"",R_input!$C33)</f>
         <v/>
       </c>
     </row>
@@ -3799,7 +3793,7 @@
         <v/>
       </c>
       <c r="B34" s="4" t="str">
-        <f>'C'!$B34</f>
+        <f>IF(R_input!$C34=0,"",R_input!$C34)</f>
         <v/>
       </c>
     </row>
@@ -3809,7 +3803,7 @@
         <v/>
       </c>
       <c r="B35" s="4" t="str">
-        <f>'C'!$B35</f>
+        <f>IF(R_input!$C35=0,"",R_input!$C35)</f>
         <v/>
       </c>
     </row>
@@ -3819,7 +3813,7 @@
         <v/>
       </c>
       <c r="B36" s="4" t="str">
-        <f>'C'!$B36</f>
+        <f>IF(R_input!$C36=0,"",R_input!$C36)</f>
         <v/>
       </c>
     </row>
@@ -3829,7 +3823,7 @@
         <v/>
       </c>
       <c r="B37" s="4" t="str">
-        <f>'C'!$B37</f>
+        <f>IF(R_input!$C37=0,"",R_input!$C37)</f>
         <v/>
       </c>
     </row>
@@ -3839,7 +3833,7 @@
         <v/>
       </c>
       <c r="B38" s="4" t="str">
-        <f>'C'!$B38</f>
+        <f>IF(R_input!$C38=0,"",R_input!$C38)</f>
         <v/>
       </c>
     </row>
@@ -3849,7 +3843,7 @@
         <v/>
       </c>
       <c r="B39" s="4" t="str">
-        <f>'C'!$B39</f>
+        <f>IF(R_input!$C39=0,"",R_input!$C39)</f>
         <v/>
       </c>
     </row>
@@ -3859,7 +3853,7 @@
         <v/>
       </c>
       <c r="B40" s="4" t="str">
-        <f>'C'!$B40</f>
+        <f>IF(R_input!$C40=0,"",R_input!$C40)</f>
         <v/>
       </c>
     </row>
@@ -3869,7 +3863,7 @@
         <v/>
       </c>
       <c r="B41" s="4" t="str">
-        <f>'C'!$B41</f>
+        <f>IF(R_input!$C41=0,"",R_input!$C41)</f>
         <v/>
       </c>
     </row>
@@ -3879,7 +3873,7 @@
         <v/>
       </c>
       <c r="B42" s="4" t="str">
-        <f>'C'!$B42</f>
+        <f>IF(R_input!$C42=0,"",R_input!$C42)</f>
         <v/>
       </c>
     </row>
@@ -3889,7 +3883,7 @@
         <v/>
       </c>
       <c r="B43" s="4" t="str">
-        <f>'C'!$B43</f>
+        <f>IF(R_input!$C43=0,"",R_input!$C43)</f>
         <v/>
       </c>
     </row>
@@ -3899,7 +3893,7 @@
         <v/>
       </c>
       <c r="B44" s="4" t="str">
-        <f>'C'!$B44</f>
+        <f>IF(R_input!$C44=0,"",R_input!$C44)</f>
         <v/>
       </c>
     </row>
@@ -3909,7 +3903,7 @@
         <v/>
       </c>
       <c r="B45" s="4" t="str">
-        <f>'C'!$B45</f>
+        <f>IF(R_input!$C45=0,"",R_input!$C45)</f>
         <v/>
       </c>
     </row>
@@ -3919,7 +3913,7 @@
         <v/>
       </c>
       <c r="B46" s="4" t="str">
-        <f>'C'!$B46</f>
+        <f>IF(R_input!$C46=0,"",R_input!$C46)</f>
         <v/>
       </c>
     </row>
@@ -3929,7 +3923,7 @@
         <v/>
       </c>
       <c r="B47" s="4" t="str">
-        <f>'C'!$B47</f>
+        <f>IF(R_input!$C47=0,"",R_input!$C47)</f>
         <v/>
       </c>
     </row>
@@ -3939,7 +3933,7 @@
         <v/>
       </c>
       <c r="B48" s="4" t="str">
-        <f>'C'!$B48</f>
+        <f>IF(R_input!$C48=0,"",R_input!$C48)</f>
         <v/>
       </c>
     </row>
@@ -3949,7 +3943,7 @@
         <v/>
       </c>
       <c r="B49" s="4" t="str">
-        <f>'C'!$B49</f>
+        <f>IF(R_input!$C49=0,"",R_input!$C49)</f>
         <v/>
       </c>
     </row>
@@ -3959,7 +3953,7 @@
         <v/>
       </c>
       <c r="B50" s="4" t="str">
-        <f>'C'!$B50</f>
+        <f>IF(R_input!$C50=0,"",R_input!$C50)</f>
         <v/>
       </c>
     </row>
@@ -3969,7 +3963,7 @@
         <v/>
       </c>
       <c r="B51" s="4" t="str">
-        <f>'C'!$B51</f>
+        <f>IF(R_input!$C51=0,"",R_input!$C51)</f>
         <v/>
       </c>
     </row>
@@ -3979,7 +3973,7 @@
         <v/>
       </c>
       <c r="B52" s="4" t="str">
-        <f>'C'!$B52</f>
+        <f>IF(R_input!$C52=0,"",R_input!$C52)</f>
         <v/>
       </c>
     </row>
@@ -3989,7 +3983,7 @@
         <v/>
       </c>
       <c r="B53" s="4" t="str">
-        <f>'C'!$B53</f>
+        <f>IF(R_input!$C53=0,"",R_input!$C53)</f>
         <v/>
       </c>
     </row>
@@ -3999,7 +3993,7 @@
         <v/>
       </c>
       <c r="B54" s="4" t="str">
-        <f>'C'!$B54</f>
+        <f>IF(R_input!$C54=0,"",R_input!$C54)</f>
         <v/>
       </c>
     </row>
@@ -4009,7 +4003,7 @@
         <v/>
       </c>
       <c r="B55" s="4" t="str">
-        <f>'C'!$B55</f>
+        <f>IF(R_input!$C55=0,"",R_input!$C55)</f>
         <v/>
       </c>
     </row>
@@ -4019,7 +4013,7 @@
         <v/>
       </c>
       <c r="B56" s="4" t="str">
-        <f>'C'!$B56</f>
+        <f>IF(R_input!$C56=0,"",R_input!$C56)</f>
         <v/>
       </c>
     </row>
@@ -4029,7 +4023,7 @@
         <v/>
       </c>
       <c r="B57" s="4" t="str">
-        <f>'C'!$B57</f>
+        <f>IF(R_input!$C57=0,"",R_input!$C57)</f>
         <v/>
       </c>
     </row>
@@ -4039,7 +4033,7 @@
         <v/>
       </c>
       <c r="B58" s="4" t="str">
-        <f>'C'!$B58</f>
+        <f>IF(R_input!$C58=0,"",R_input!$C58)</f>
         <v/>
       </c>
     </row>
@@ -4049,7 +4043,7 @@
         <v/>
       </c>
       <c r="B59" s="4" t="str">
-        <f>'C'!$B59</f>
+        <f>IF(R_input!$C59=0,"",R_input!$C59)</f>
         <v/>
       </c>
     </row>
@@ -4059,7 +4053,7 @@
         <v/>
       </c>
       <c r="B60" s="4" t="str">
-        <f>'C'!$B60</f>
+        <f>IF(R_input!$C60=0,"",R_input!$C60)</f>
         <v/>
       </c>
     </row>
@@ -5806,17 +5800,17 @@
         <f>IF('C'!$A1="","",'C'!$A1&amp;"init")</f>
         <v xml:space="preserve"> k1init</v>
       </c>
-      <c r="B1" s="4">
+      <c r="B1" s="4" t="str">
         <f>'C'!$B1</f>
-        <v>10000</v>
+        <v xml:space="preserve"> k1init</v>
       </c>
       <c r="D1" t="str">
         <f>IF(NOT(AND(F1,E1)),"",'C'!$A1&amp;"init")</f>
-        <v xml:space="preserve"> k1init</v>
-      </c>
-      <c r="E1">
+        <v/>
+      </c>
+      <c r="E1" t="b">
         <f>IFERROR(VALUE('C'!$B1),FALSE())</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="F1" s="12" t="b">
         <f>NOT('C'!$A1="")</f>
@@ -5828,17 +5822,17 @@
         <f>IF('C'!$A2="","",'C'!$A2&amp;"init")</f>
         <v xml:space="preserve"> k2init</v>
       </c>
-      <c r="B2" s="4">
+      <c r="B2" s="4" t="str">
         <f>'C'!$B2</f>
-        <v>10000</v>
+        <v xml:space="preserve"> k2init</v>
       </c>
       <c r="D2" t="str">
         <f>IF(NOT(AND(F2,E2)),"",'C'!$A2&amp;"init")</f>
-        <v xml:space="preserve"> k2init</v>
-      </c>
-      <c r="E2">
+        <v/>
+      </c>
+      <c r="E2" t="b">
         <f>IFERROR(VALUE('C'!$B2),FALSE())</f>
-        <v>10000</v>
+        <v>0</v>
       </c>
       <c r="F2" s="12" t="b">
         <f>NOT('C'!$A2="")</f>
@@ -5850,17 +5844,17 @@
         <f>IF('C'!$A3="","",'C'!$A3&amp;"init")</f>
         <v xml:space="preserve"> k3init</v>
       </c>
-      <c r="B3" s="4">
+      <c r="B3" s="4" t="str">
         <f>'C'!$B3</f>
-        <v>100</v>
+        <v xml:space="preserve"> k3init</v>
       </c>
       <c r="D3" t="str">
         <f>IF(NOT(AND(F3,E3)),"",'C'!$A3&amp;"init")</f>
-        <v xml:space="preserve"> k3init</v>
-      </c>
-      <c r="E3">
+        <v/>
+      </c>
+      <c r="E3" t="b">
         <f>IFERROR(VALUE('C'!$B3),FALSE())</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="F3" s="12" t="b">
         <f>NOT('C'!$A3="")</f>
@@ -5874,7 +5868,7 @@
       </c>
       <c r="B4" s="4" t="str">
         <f>'C'!$B4</f>
-        <v>K2*k5</v>
+        <v xml:space="preserve"> k4init</v>
       </c>
       <c r="D4" t="str">
         <f>IF(NOT(AND(F4,E4)),"",'C'!$A4&amp;"init")</f>
@@ -5894,17 +5888,17 @@
         <f>IF('C'!$A5="","",'C'!$A5&amp;"init")</f>
         <v xml:space="preserve"> k5init</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="4" t="str">
         <f>'C'!$B5</f>
-        <v>1E-4</v>
+        <v xml:space="preserve"> k5init</v>
       </c>
       <c r="D5" t="str">
         <f>IF(NOT(AND(F5,E5)),"",'C'!$A5&amp;"init")</f>
-        <v xml:space="preserve"> k5init</v>
-      </c>
-      <c r="E5">
+        <v/>
+      </c>
+      <c r="E5" t="b">
         <f>IFERROR(VALUE('C'!$B5),FALSE())</f>
-        <v>1E-4</v>
+        <v>0</v>
       </c>
       <c r="F5" s="12" t="b">
         <f>NOT('C'!$A5="")</f>
@@ -5916,17 +5910,17 @@
         <f>IF('C'!$A6="","",'C'!$A6&amp;"init")</f>
         <v xml:space="preserve"> k6init</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="4" t="str">
         <f>'C'!$B6</f>
-        <v>2</v>
+        <v xml:space="preserve"> k6init</v>
       </c>
       <c r="D6" t="str">
         <f>IF(NOT(AND(F6,E6)),"",'C'!$A6&amp;"init")</f>
-        <v xml:space="preserve"> k6init</v>
-      </c>
-      <c r="E6">
+        <v/>
+      </c>
+      <c r="E6" t="b">
         <f>IFERROR(VALUE('C'!$B6),FALSE())</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F6" s="12" t="b">
         <f>NOT('C'!$A6="")</f>
@@ -5940,7 +5934,7 @@
       </c>
       <c r="B7" s="4" t="str">
         <f>'C'!$B7</f>
-        <v>K4*k8</v>
+        <v xml:space="preserve"> k7init</v>
       </c>
       <c r="D7" t="str">
         <f>IF(NOT(AND(F7,E7)),"",'C'!$A7&amp;"init")</f>
@@ -5960,17 +5954,17 @@
         <f>IF('C'!$A8="","",'C'!$A8&amp;"init")</f>
         <v xml:space="preserve"> k8init</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="4" t="str">
         <f>'C'!$B8</f>
-        <v>1</v>
+        <v xml:space="preserve"> k8init</v>
       </c>
       <c r="D8" t="str">
         <f>IF(NOT(AND(F8,E8)),"",'C'!$A8&amp;"init")</f>
-        <v xml:space="preserve"> k8init</v>
-      </c>
-      <c r="E8">
+        <v/>
+      </c>
+      <c r="E8" t="b">
         <f>IFERROR(VALUE('C'!$B8),FALSE())</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F8" s="12" t="b">
         <f>NOT('C'!$A8="")</f>
@@ -5982,17 +5976,17 @@
         <f>IF('C'!$A9="","",'C'!$A9&amp;"init")</f>
         <v xml:space="preserve"> k9init</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="4" t="str">
         <f>'C'!$B9</f>
-        <v>1</v>
+        <v xml:space="preserve"> k9init</v>
       </c>
       <c r="D9" t="str">
         <f>IF(NOT(AND(F9,E9)),"",'C'!$A9&amp;"init")</f>
-        <v xml:space="preserve"> k9init</v>
-      </c>
-      <c r="E9">
+        <v/>
+      </c>
+      <c r="E9" t="b">
         <f>IFERROR(VALUE('C'!$B9),FALSE())</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F9" s="12" t="b">
         <f>NOT('C'!$A9="")</f>
@@ -6004,17 +5998,17 @@
         <f>IF('C'!$A10="","",'C'!$A10&amp;"init")</f>
         <v xml:space="preserve"> k10init</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="4" t="str">
         <f>'C'!$B10</f>
-        <v>10</v>
+        <v xml:space="preserve"> k10init</v>
       </c>
       <c r="D10" t="str">
         <f>IF(NOT(AND(F10,E10)),"",'C'!$A10&amp;"init")</f>
-        <v xml:space="preserve"> k10init</v>
-      </c>
-      <c r="E10">
+        <v/>
+      </c>
+      <c r="E10" t="b">
         <f>IFERROR(VALUE('C'!$B10),FALSE())</f>
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F10" s="12" t="b">
         <f>NOT('C'!$A10="")</f>
@@ -6026,17 +6020,17 @@
         <f>IF('C'!$A11="","",'C'!$A11&amp;"init")</f>
         <v xml:space="preserve"> k11init</v>
       </c>
-      <c r="B11" s="4">
+      <c r="B11" s="4" t="str">
         <f>'C'!$B11</f>
-        <v>1</v>
+        <v xml:space="preserve"> k11init</v>
       </c>
       <c r="D11" t="str">
         <f>IF(NOT(AND(F11,E11)),"",'C'!$A11&amp;"init")</f>
-        <v xml:space="preserve"> k11init</v>
-      </c>
-      <c r="E11">
+        <v/>
+      </c>
+      <c r="E11" t="b">
         <f>IFERROR(VALUE('C'!$B11),FALSE())</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F11" s="12" t="b">
         <f>NOT('C'!$A11="")</f>
@@ -6048,17 +6042,17 @@
         <f>IF('C'!$A12="","",'C'!$A12&amp;"init")</f>
         <v>K2init</v>
       </c>
-      <c r="B12" s="4">
+      <c r="B12" s="4" t="str">
         <f>'C'!$B12</f>
-        <v>100000</v>
+        <v>K2init</v>
       </c>
       <c r="D12" t="str">
         <f>IF(NOT(AND(F12,E12)),"",'C'!$A12&amp;"init")</f>
-        <v>K2init</v>
-      </c>
-      <c r="E12">
+        <v/>
+      </c>
+      <c r="E12" t="b">
         <f>IFERROR(VALUE('C'!$B12),FALSE())</f>
-        <v>100000</v>
+        <v>0</v>
       </c>
       <c r="F12" s="12" t="b">
         <f>NOT('C'!$A12="")</f>
@@ -6070,17 +6064,17 @@
         <f>IF('C'!$A13="","",'C'!$A13&amp;"init")</f>
         <v>K4init</v>
       </c>
-      <c r="B13" s="4">
+      <c r="B13" s="4" t="str">
         <f>'C'!$B13</f>
-        <v>0.05</v>
+        <v>K4init</v>
       </c>
       <c r="D13" t="str">
         <f>IF(NOT(AND(F13,E13)),"",'C'!$A13&amp;"init")</f>
-        <v>K4init</v>
-      </c>
-      <c r="E13">
+        <v/>
+      </c>
+      <c r="E13" t="b">
         <f>IFERROR(VALUE('C'!$B13),FALSE())</f>
-        <v>0.05</v>
+        <v>0</v>
       </c>
       <c r="F13" s="12" t="b">
         <f>NOT('C'!$A13="")</f>

</xml_diff>